<commit_message>
small data  reorganization and plot improvements
</commit_message>
<xml_diff>
--- a/data/date_temp.xlsx
+++ b/data/date_temp.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\movealong\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="8_{6A5C9D6E-1683-4F6F-9D5E-28DBA0008C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19554C03-E38E-4C7A-930B-DCCDDEE7B51D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6D779A2-57FD-4F87-824F-575DB36B2135}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="weekly_Eduardo" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,16 +60,16 @@
     <t>date</t>
   </si>
   <si>
-    <t>condition</t>
+    <t>regime</t>
   </si>
   <si>
-    <t>regime</t>
+    <t>incubator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,11 +415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F56D3FB-B327-4595-B707-9F52643A00D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G862"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +439,10 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -22020,7 +22019,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:G798">
+  <sortState ref="A5:G798">
     <sortCondition ref="B5:B798"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>